<commit_message>
changed test excel format
</commit_message>
<xml_diff>
--- a/jonahAdds/Book1.xlsx
+++ b/jonahAdds/Book1.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jonah\School\ASI\bloom\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jonah\School\ASI\bloom\BBMap\jonahAdds\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{5FBA5924-EB2E-4344-9808-18C3E8C2B231}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{805E0287-0FD9-4D3B-94E2-4EB2088F3C5A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" xr2:uid="{01E1030F-6651-4350-9E2D-F1EB30A76327}"/>
   </bookViews>
@@ -35,19 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="83">
-  <si>
-    <t>Sequence</t>
-  </si>
-  <si>
-    <t>Count</t>
-  </si>
-  <si>
-    <t>Percentage</t>
-  </si>
-  <si>
-    <t>Possible Source</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="79">
   <si>
     <t>CCTTAGGCAACCTGGTGGTCCCCCGCTCCCGGGAGGTCACCATATTGATG</t>
   </si>
@@ -635,10 +623,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{809F5894-81A2-466A-897D-6E5D3C40FDF6}">
-  <dimension ref="A1:D79"/>
+  <dimension ref="A1:D78"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:D79"/>
+      <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -647,1106 +635,1092 @@
       <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
+      <c r="B1">
+        <v>36572</v>
+      </c>
+      <c r="C1">
+        <v>1.25115889225295</v>
       </c>
       <c r="D1" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B2">
-        <v>36572</v>
+        <v>32218</v>
       </c>
       <c r="C2">
-        <v>1.25115889225295</v>
+        <v>1.1022048887292299</v>
       </c>
       <c r="D2" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="B3">
-        <v>32218</v>
+        <v>28643</v>
       </c>
       <c r="C3">
-        <v>1.1022048887292299</v>
+        <v>0.97990113066830797</v>
       </c>
       <c r="D3" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="B4">
-        <v>28643</v>
+        <v>23280</v>
       </c>
       <c r="C4">
-        <v>0.97990113066830797</v>
+        <v>0.79642838815620598</v>
       </c>
       <c r="D4" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="B5">
-        <v>23280</v>
+        <v>17582</v>
       </c>
       <c r="C5">
-        <v>0.79642838815620598</v>
+        <v>0.60149501376986303</v>
       </c>
       <c r="D5" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="B6">
-        <v>17582</v>
+        <v>17523</v>
       </c>
       <c r="C6">
-        <v>0.60149501376986303</v>
+        <v>0.59947657412634003</v>
       </c>
       <c r="D6" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="B7">
-        <v>17523</v>
+        <v>16848</v>
       </c>
       <c r="C7">
-        <v>0.59947657412634003</v>
+        <v>0.57638425617078004</v>
       </c>
       <c r="D7" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="B8">
-        <v>16848</v>
+        <v>16720</v>
       </c>
       <c r="C8">
-        <v>0.57638425617078004</v>
+        <v>0.572005268469578</v>
       </c>
       <c r="D8" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="B9">
-        <v>16720</v>
+        <v>14675</v>
       </c>
       <c r="C9">
-        <v>0.572005268469578</v>
+        <v>0.50204409777458403</v>
       </c>
       <c r="D9" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="B10">
-        <v>14675</v>
+        <v>14649</v>
       </c>
       <c r="C10">
-        <v>0.50204409777458403</v>
+        <v>0.50115461589777799</v>
       </c>
       <c r="D10" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="B11">
-        <v>14649</v>
+        <v>13859</v>
       </c>
       <c r="C11">
-        <v>0.50115461589777799</v>
+        <v>0.47412805117941798</v>
       </c>
       <c r="D11" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="B12">
-        <v>13859</v>
+        <v>13293</v>
       </c>
       <c r="C12">
-        <v>0.47412805117941798</v>
+        <v>0.45476471493816301</v>
       </c>
       <c r="D12" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="B13">
-        <v>13293</v>
+        <v>13187</v>
       </c>
       <c r="C13">
-        <v>0.45476471493816301</v>
+        <v>0.45113836574810501</v>
       </c>
       <c r="D13" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B14">
-        <v>13187</v>
+        <v>12971</v>
       </c>
       <c r="C14">
-        <v>0.45113836574810501</v>
+        <v>0.44374882400232601</v>
       </c>
       <c r="D14" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="B15">
-        <v>12971</v>
+        <v>12829</v>
       </c>
       <c r="C15">
-        <v>0.44374882400232601</v>
+        <v>0.43889088452130398</v>
       </c>
       <c r="D15" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B16">
-        <v>12829</v>
+        <v>12682</v>
       </c>
       <c r="C16">
-        <v>0.43889088452130398</v>
+        <v>0.43386189083320498</v>
       </c>
       <c r="D16" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B17">
-        <v>12682</v>
+        <v>12531</v>
       </c>
       <c r="C17">
-        <v>0.43386189083320498</v>
+        <v>0.42869605377944198</v>
       </c>
       <c r="D17" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B18">
-        <v>12531</v>
+        <v>12467</v>
       </c>
       <c r="C18">
-        <v>0.42869605377944198</v>
+        <v>0.42650655992884101</v>
       </c>
       <c r="D18" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="B19">
-        <v>12467</v>
+        <v>12168</v>
       </c>
       <c r="C19">
-        <v>0.42650655992884101</v>
+        <v>0.41627751834556298</v>
       </c>
       <c r="D19" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B20">
-        <v>12168</v>
+        <v>12127</v>
       </c>
       <c r="C20">
-        <v>0.41627751834556298</v>
+        <v>0.41487487384752197</v>
       </c>
       <c r="D20" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B21">
-        <v>12127</v>
+        <v>12075</v>
       </c>
       <c r="C21">
-        <v>0.41487487384752197</v>
+        <v>0.413095910093908</v>
       </c>
       <c r="D21" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B22">
-        <v>12075</v>
+        <v>10929</v>
       </c>
       <c r="C22">
-        <v>0.413095910093908</v>
+        <v>0.37389028583158002</v>
       </c>
       <c r="D22" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="B23">
-        <v>10929</v>
+        <v>10553</v>
       </c>
       <c r="C23">
-        <v>0.37389028583158002</v>
+        <v>0.361027009459297</v>
       </c>
       <c r="D23" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B24">
-        <v>10553</v>
+        <v>10545</v>
       </c>
       <c r="C24">
-        <v>0.361027009459297</v>
+        <v>0.360753322727972</v>
       </c>
       <c r="D24" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B25">
-        <v>10545</v>
+        <v>10490</v>
       </c>
       <c r="C25">
-        <v>0.360753322727972</v>
+        <v>0.35887172645011201</v>
       </c>
       <c r="D25" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="B26">
-        <v>10490</v>
+        <v>10074</v>
       </c>
       <c r="C26">
-        <v>0.35887172645011201</v>
+        <v>0.34464001642120301</v>
       </c>
       <c r="D26" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="B27">
-        <v>10074</v>
+        <v>10045</v>
       </c>
       <c r="C27">
-        <v>0.34464001642120301</v>
+        <v>0.34364790202015</v>
       </c>
       <c r="D27" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="B28">
-        <v>10045</v>
+        <v>9863</v>
       </c>
       <c r="C28">
-        <v>0.34364790202015</v>
+        <v>0.33742152888250199</v>
       </c>
       <c r="D28" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="B29">
-        <v>9863</v>
+        <v>9819</v>
       </c>
       <c r="C29">
-        <v>0.33742152888250199</v>
+        <v>0.33591625186021401</v>
       </c>
       <c r="D29" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="B30">
-        <v>9819</v>
+        <v>9314</v>
       </c>
       <c r="C30">
-        <v>0.33591625186021401</v>
+        <v>0.31863977694531398</v>
       </c>
       <c r="D30" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="B31">
-        <v>9314</v>
+        <v>9225</v>
       </c>
       <c r="C31">
-        <v>0.31863977694531398</v>
+        <v>0.315595012059321</v>
       </c>
       <c r="D31" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="B32">
-        <v>9225</v>
+        <v>9116</v>
       </c>
       <c r="C32">
-        <v>0.315595012059321</v>
+        <v>0.31186603034501598</v>
       </c>
       <c r="D32" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="B33">
-        <v>9116</v>
+        <v>8965</v>
       </c>
       <c r="C33">
-        <v>0.31186603034501598</v>
+        <v>0.30670019329125398</v>
       </c>
       <c r="D33" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="B34">
-        <v>8965</v>
+        <v>8757</v>
       </c>
       <c r="C34">
-        <v>0.30670019329125398</v>
+        <v>0.29958433827679898</v>
       </c>
       <c r="D34" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="B35">
-        <v>8757</v>
+        <v>8750</v>
       </c>
       <c r="C35">
-        <v>0.29958433827679898</v>
+        <v>0.29934486238689001</v>
       </c>
       <c r="D35" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="B36">
-        <v>8750</v>
+        <v>8629</v>
       </c>
       <c r="C36">
-        <v>0.29934486238689001</v>
+        <v>0.29520535057559699</v>
       </c>
       <c r="D36" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="B37">
-        <v>8629</v>
+        <v>8010</v>
       </c>
       <c r="C37">
-        <v>0.29520535057559699</v>
+        <v>0.27402883973931302</v>
       </c>
       <c r="D37" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B38">
-        <v>8010</v>
+        <v>8007</v>
       </c>
       <c r="C38">
-        <v>0.27402883973931302</v>
+        <v>0.273926207215066</v>
       </c>
       <c r="D38" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="B39">
-        <v>8007</v>
+        <v>7727</v>
       </c>
       <c r="C39">
-        <v>0.273926207215066</v>
+        <v>0.26434717161868498</v>
       </c>
       <c r="D39" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="B40">
-        <v>7727</v>
+        <v>7692</v>
       </c>
       <c r="C40">
-        <v>0.26434717161868498</v>
+        <v>0.26314979216913797</v>
       </c>
       <c r="D40" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="B41">
-        <v>7692</v>
+        <v>7199</v>
       </c>
       <c r="C41">
-        <v>0.26314979216913797</v>
+        <v>0.24628384735122499</v>
       </c>
       <c r="D41" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B42">
-        <v>7199</v>
+        <v>6978</v>
       </c>
       <c r="C42">
-        <v>0.24628384735122499</v>
+        <v>0.238723251398368</v>
       </c>
       <c r="D42" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="B43">
-        <v>6978</v>
+        <v>6962</v>
       </c>
       <c r="C43">
-        <v>0.238723251398368</v>
+        <v>0.23817587793571701</v>
       </c>
       <c r="D43" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="B44">
-        <v>6962</v>
+        <v>6900</v>
       </c>
       <c r="C44">
-        <v>0.23817587793571701</v>
+        <v>0.23605480576794699</v>
       </c>
       <c r="D44" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="B45">
-        <v>6900</v>
+        <v>6824</v>
       </c>
       <c r="C45">
-        <v>0.23605480576794699</v>
+        <v>0.233454781820358</v>
       </c>
       <c r="D45" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="B46">
-        <v>6824</v>
+        <v>6733</v>
       </c>
       <c r="C46">
-        <v>0.233454781820358</v>
+        <v>0.230341595251535</v>
       </c>
       <c r="D46" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="B47">
-        <v>6733</v>
+        <v>6707</v>
       </c>
       <c r="C47">
-        <v>0.230341595251535</v>
+        <v>0.22945211337472801</v>
       </c>
       <c r="D47" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="B48">
-        <v>6707</v>
+        <v>6642</v>
       </c>
       <c r="C48">
-        <v>0.22945211337472801</v>
+        <v>0.22722840868271099</v>
       </c>
       <c r="D48" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="B49">
-        <v>6642</v>
+        <v>6578</v>
       </c>
       <c r="C49">
-        <v>0.22722840868271099</v>
+        <v>0.22503891483211</v>
       </c>
       <c r="D49" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="B50">
-        <v>6578</v>
+        <v>6371</v>
       </c>
       <c r="C50">
-        <v>0.22503891483211</v>
+        <v>0.217957270659071</v>
       </c>
       <c r="D50" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="B51">
-        <v>6371</v>
+        <v>6014</v>
       </c>
       <c r="C51">
-        <v>0.217957270659071</v>
+        <v>0.205744000273686</v>
       </c>
       <c r="D51" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="B52">
-        <v>6014</v>
+        <v>5899</v>
       </c>
       <c r="C52">
-        <v>0.205744000273686</v>
+        <v>0.20180975351088701</v>
       </c>
       <c r="D52" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="B53">
-        <v>5899</v>
+        <v>5824</v>
       </c>
       <c r="C53">
-        <v>0.20180975351088701</v>
+        <v>0.19924394040471399</v>
       </c>
       <c r="D53" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="B54">
-        <v>5824</v>
+        <v>5560</v>
       </c>
       <c r="C54">
-        <v>0.19924394040471399</v>
+        <v>0.190212278270984</v>
       </c>
       <c r="D54" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="B55">
-        <v>5560</v>
+        <v>5449</v>
       </c>
       <c r="C55">
-        <v>0.190212278270984</v>
+        <v>0.186414874873847</v>
       </c>
       <c r="D55" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="B56">
-        <v>5449</v>
+        <v>5208</v>
       </c>
       <c r="C56">
-        <v>0.186414874873847</v>
+        <v>0.178170062092677</v>
       </c>
       <c r="D56" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="B57">
-        <v>5208</v>
+        <v>5110</v>
       </c>
       <c r="C57">
-        <v>0.178170062092677</v>
+        <v>0.17481739963394399</v>
       </c>
       <c r="D57" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="B58">
-        <v>5110</v>
+        <v>5048</v>
       </c>
       <c r="C58">
-        <v>0.17481739963394399</v>
+        <v>0.172696327466174</v>
       </c>
       <c r="D58" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="B59">
-        <v>5048</v>
+        <v>5041</v>
       </c>
       <c r="C59">
-        <v>0.172696327466174</v>
+        <v>0.172456851576264</v>
       </c>
       <c r="D59" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="B60">
-        <v>5041</v>
+        <v>5006</v>
       </c>
       <c r="C60">
-        <v>0.172456851576264</v>
+        <v>0.17125947212671599</v>
       </c>
       <c r="D60" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="B61">
-        <v>5006</v>
+        <v>4992</v>
       </c>
       <c r="C61">
-        <v>0.17125947212671599</v>
+        <v>0.170780520346897</v>
       </c>
       <c r="D61" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="B62">
-        <v>4992</v>
+        <v>4754</v>
       </c>
       <c r="C62">
-        <v>0.170780520346897</v>
+        <v>0.16263834008997399</v>
       </c>
       <c r="D62" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="B63">
-        <v>4754</v>
+        <v>4702</v>
       </c>
       <c r="C63">
-        <v>0.16263834008997399</v>
+        <v>0.16085937633636099</v>
       </c>
       <c r="D63" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="B64">
-        <v>4702</v>
+        <v>4574</v>
       </c>
       <c r="C64">
-        <v>0.16085937633636099</v>
+        <v>0.15648038863515801</v>
       </c>
       <c r="D64" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="B65">
-        <v>4574</v>
+        <v>4478</v>
       </c>
       <c r="C65">
-        <v>0.15648038863515801</v>
+        <v>0.153196147859256</v>
       </c>
       <c r="D65" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="B66">
-        <v>4478</v>
+        <v>4432</v>
       </c>
       <c r="C66">
-        <v>0.153196147859256</v>
+        <v>0.151622449154136</v>
       </c>
       <c r="D66" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="B67">
-        <v>4432</v>
+        <v>4167</v>
       </c>
       <c r="C67">
-        <v>0.151622449154136</v>
+        <v>0.14255657617899101</v>
       </c>
       <c r="D67" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="B68">
-        <v>4167</v>
+        <v>4098</v>
       </c>
       <c r="C68">
-        <v>0.14255657617899101</v>
+        <v>0.14019602812131099</v>
       </c>
       <c r="D68" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="B69">
-        <v>4098</v>
+        <v>4095</v>
       </c>
       <c r="C69">
-        <v>0.14019602812131099</v>
+        <v>0.14009339559706399</v>
       </c>
       <c r="D69" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="B70">
-        <v>4095</v>
+        <v>3928</v>
       </c>
       <c r="C70">
-        <v>0.14009339559706399</v>
+        <v>0.134380185080652</v>
       </c>
       <c r="D70" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="B71">
-        <v>3928</v>
+        <v>3811</v>
       </c>
       <c r="C71">
-        <v>0.134380185080652</v>
+        <v>0.13037751663502101</v>
       </c>
       <c r="D71" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="B72">
-        <v>3811</v>
+        <v>3758</v>
       </c>
       <c r="C72">
-        <v>0.13037751663502101</v>
+        <v>0.12856434203999201</v>
       </c>
       <c r="D72" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="B73">
-        <v>3758</v>
+        <v>3721</v>
       </c>
       <c r="C73">
-        <v>0.12856434203999201</v>
+        <v>0.127298540907613</v>
       </c>
       <c r="D73" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="B74">
-        <v>3721</v>
+        <v>3647</v>
       </c>
       <c r="C74">
-        <v>0.127298540907613</v>
+        <v>0.124766938642855</v>
       </c>
       <c r="D74" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B75">
-        <v>3647</v>
+        <v>3641</v>
       </c>
       <c r="C75">
-        <v>0.124766938642855</v>
+        <v>0.124561673594362</v>
       </c>
       <c r="D75" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="B76">
-        <v>3641</v>
+        <v>3629</v>
       </c>
       <c r="C76">
-        <v>0.124561673594362</v>
+        <v>0.12415114349737399</v>
       </c>
       <c r="D76" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="B77">
-        <v>3629</v>
+        <v>3505</v>
       </c>
       <c r="C77">
-        <v>0.12415114349737399</v>
+        <v>0.11990899916183401</v>
       </c>
       <c r="D77" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="B78">
-        <v>3505</v>
+        <v>3382</v>
       </c>
       <c r="C78">
-        <v>0.11990899916183401</v>
+        <v>0.11570106566771</v>
       </c>
       <c r="D78" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A79" t="s">
-        <v>82</v>
-      </c>
-      <c r="B79">
-        <v>3382</v>
-      </c>
-      <c r="C79">
-        <v>0.11570106566771</v>
-      </c>
-      <c r="D79" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>